<commit_message>
many changes in framework
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{38FC9B5D-85BC-47D2-83B8-041D124074CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E621492-4BBE-4542-91B7-51679759DFB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19460" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19460" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredentials" sheetId="2" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>retrixsingh01@gmail.com</t>
   </si>
   <si>
-    <t>Retrix123#</t>
-  </si>
-  <si>
     <t>Retrix</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>RetrixAlpha</t>
+  </si>
+  <si>
+    <t>UmV0cml4MTIzIw</t>
   </si>
 </sst>
 </file>
@@ -414,13 +414,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.54296875" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" customWidth="1"/>
     <col min="4" max="4" width="16.7265625" customWidth="1"/>
   </cols>
@@ -444,27 +444,27 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>